<commit_message>
Update to god roll excel sheet
</commit_message>
<xml_diff>
--- a/God Rolls.xlsx
+++ b/God Rolls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Destiny Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C4824D-2D3A-4FFA-BF31-D5FE4823D301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{39037BA0-6309-4957-A9A0-6F4E166A17ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="5070" windowWidth="21600" windowHeight="15435" xr2:uid="{68E4B836-756E-4019-AEFC-B535E69C91C4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Chroma Rush</t>
   </si>
   <si>
-    <t>Compass Rose</t>
-  </si>
-  <si>
     <t>Corrective Measure</t>
   </si>
   <si>
@@ -243,9 +240,6 @@
     <t>Feeding Frenzy</t>
   </si>
   <si>
-    <t>Armour-Piercing Rounds</t>
-  </si>
-  <si>
     <t>Appended Mag</t>
   </si>
   <si>
@@ -319,6 +313,63 @@
   </si>
   <si>
     <t>Fastdraw HCS</t>
+  </si>
+  <si>
+    <t>*Compass Rose</t>
+  </si>
+  <si>
+    <t>rifled barrel</t>
+  </si>
+  <si>
+    <t>assault mag</t>
+  </si>
+  <si>
+    <t>slideshot</t>
+  </si>
+  <si>
+    <t>opening shot</t>
+  </si>
+  <si>
+    <t>Armor-Piercing Rounds</t>
+  </si>
+  <si>
+    <t>Lasting Impression</t>
+  </si>
+  <si>
+    <t>Alloy Casing</t>
+  </si>
+  <si>
+    <t>Confined Launch</t>
+  </si>
+  <si>
+    <t>Rapid Hit</t>
+  </si>
+  <si>
+    <t>Quick Launch</t>
+  </si>
+  <si>
+    <t>Chain Reaction</t>
+  </si>
+  <si>
+    <t>Impulse Amplified</t>
+  </si>
+  <si>
+    <t>Clown Cartridge</t>
+  </si>
+  <si>
+    <t>Opening Shot</t>
+  </si>
+  <si>
+    <t>Snapshot Sights</t>
+  </si>
+  <si>
+    <t>Reservoir Burst</t>
+  </si>
+  <si>
+    <t>Liquid Coils</t>
+  </si>
+  <si>
+    <t>Under Pressure</t>
   </si>
 </sst>
 </file>
@@ -394,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -403,6 +454,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38F4BD20-7028-445C-8DD5-CF386C352D58}">
-  <dimension ref="A1:F191"/>
+  <dimension ref="A1:F230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="G108" sqref="G108"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +781,7 @@
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
@@ -759,104 +811,104 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
         <v>63</v>
       </c>
-      <c r="D6" t="s">
-        <v>64</v>
-      </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -864,461 +916,462 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
         <v>67</v>
       </c>
-      <c r="D8" t="s">
-        <v>68</v>
-      </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" t="s">
-        <v>65</v>
+      <c r="D10" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" t="s">
         <v>69</v>
       </c>
-      <c r="D12" t="s">
-        <v>71</v>
-      </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" t="s">
         <v>69</v>
       </c>
-      <c r="D15" t="s">
-        <v>71</v>
-      </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" t="s">
         <v>70</v>
       </c>
-      <c r="D16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" t="s">
-        <v>72</v>
-      </c>
       <c r="F16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
         <v>67</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E17" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" t="s">
-        <v>65</v>
+      <c r="D19" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" t="s">
         <v>69</v>
       </c>
-      <c r="D21" t="s">
-        <v>71</v>
-      </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
         <v>69</v>
       </c>
-      <c r="D24" t="s">
-        <v>71</v>
-      </c>
       <c r="E24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" t="s">
         <v>70</v>
       </c>
-      <c r="D25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" t="s">
-        <v>72</v>
-      </c>
       <c r="F25" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" t="s">
         <v>67</v>
       </c>
-      <c r="D26" t="s">
-        <v>68</v>
-      </c>
       <c r="E26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" t="s">
         <v>69</v>
       </c>
-      <c r="D30" t="s">
-        <v>71</v>
-      </c>
       <c r="E30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" t="s">
         <v>69</v>
       </c>
-      <c r="D33" t="s">
-        <v>71</v>
-      </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="F34" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1326,1561 +1379,2521 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" t="s">
-        <v>70</v>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D43" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D52" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>55</v>
-      </c>
-      <c r="C57" t="s">
-        <v>74</v>
+      <c r="A57" s="8"/>
+      <c r="B57" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C60" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C65" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="E65" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="8"/>
       <c r="B68" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C68" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="E68" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C71" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D71" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D71" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="E71" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C74" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="E74" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="8"/>
       <c r="B75" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C77" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D77" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="E77" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C80" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D80" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D80" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="E80" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C81" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E81" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="F81" s="7"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C86" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="8"/>
+      <c r="B87" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B87" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="E87" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E88" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C89" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D89" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D89" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="E89" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E92" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="8"/>
+      <c r="B93" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C93" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F92" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B93" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="D93" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="95" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B97" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F97" s="3"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="99" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="8"/>
       <c r="B101" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>77</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F101" s="8"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B102" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="103" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E108" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="8"/>
+      <c r="B109" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B109" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="C109" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B110" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B112" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C112" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="8"/>
+      <c r="B113" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B114" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B115" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B116" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B117" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B118" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>18</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B121" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B122" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E123" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F123" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B125" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B126" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F127" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>20</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="8"/>
+      <c r="B129" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B130" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B131" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B132" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B133" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B134" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F135" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>21</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B137" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B138" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>22</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B141" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B142" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B143" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E143" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>23</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B145" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B146" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B147" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B148" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B149" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B150" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B151" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B152" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B153" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B154" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B155" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D155" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E155" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>24</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B157" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B158" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B159" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B160" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B161" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B162" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B163" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B164" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B165" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B166" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B167" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C167" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E167" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>25</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B169" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B170" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B171" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C171" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D171" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E171" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>26</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B173" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F173" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B174" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D174" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E174" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F174" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>28</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B177" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F177" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B178" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B179" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C179" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D179" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E179" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F179" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>29</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D180" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D112" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E112" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B113" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B114" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B115" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B116" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B117" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B118" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D119" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E119" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="E180" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D181" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F181" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>49</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">
-    <sortCondition ref="B2:B7"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:F16">
+    <sortCondition ref="B8:B16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>